<commit_message>
Updated to correct issue with message-box generation during error handling; Ran administrative update.
</commit_message>
<xml_diff>
--- a/Mars Photos - Details - Curiosity_2015_Part2.xlsx
+++ b/Mars Photos - Details - Curiosity_2015_Part2.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Details" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Details!$A$3:$E$11838</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Details!$A$3:$E$11852</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Details!$1:$3</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1340,7 +1340,7 @@
     <t>http://mars.jpl.nasa.gov/msl-raw-images/msss/00855/mcam/0855MR0037760000501034C02_DXXX.jpg</t>
   </si>
   <si>
-    <t>PHOTOS TAKEN BY MARS ROVER 'CURIOSITY' - Year 2015, Part 2 of 2 (as of 12-Sep-2024 @ 02:53 PM)</t>
+    <t>PHOTOS TAKEN BY MARS ROVER 'CURIOSITY' - Year 2015, Part 2 of 2 (as of 25-Sep-2024 @ 11:17 PM)</t>
   </si>
 </sst>
 </file>
@@ -6663,7 +6663,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:E11838"/>
+  <autoFilter ref="A3:E11852"/>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>

</xml_diff>

<commit_message>
Updated to improve error handling at web routes; Ran administrative update.
</commit_message>
<xml_diff>
--- a/Mars Photos - Details - Curiosity_2015_Part2.xlsx
+++ b/Mars Photos - Details - Curiosity_2015_Part2.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Details" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Details!$A$3:$E$11852</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Details!$A$3:$E$11854</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Details!$1:$3</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1340,7 +1340,7 @@
     <t>http://mars.jpl.nasa.gov/msl-raw-images/msss/00855/mcam/0855MR0037760000501034C02_DXXX.jpg</t>
   </si>
   <si>
-    <t>PHOTOS TAKEN BY MARS ROVER 'CURIOSITY' - Year 2015, Part 2 of 2 (as of 25-Sep-2024 @ 11:17 PM)</t>
+    <t>PHOTOS TAKEN BY MARS ROVER 'CURIOSITY' - Year 2015, Part 2 of 2 (as of 28-Sep-2024 @ 03:08 PM)</t>
   </si>
 </sst>
 </file>
@@ -6663,7 +6663,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:E11852"/>
+  <autoFilter ref="A3:E11854"/>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>

</xml_diff>